<commit_message>
Neural Network for price prediction created and optimized Linear and Logistic Regression optimized
</commit_message>
<xml_diff>
--- a/resources/btc_corr_table.xlsx
+++ b/resources/btc_corr_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Adj Close</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Volume</t>
         </is>
       </c>
@@ -470,16 +475,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.999409687677597</v>
+        <v>0.9994160075792081</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9988429929255541</v>
+        <v>0.9988591541715838</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9985279217658934</v>
+        <v>0.9985406712857549</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6669808006009431</v>
+        <v>0.9985406712857549</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.6642954180740478</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.999409687677597</v>
+        <v>0.9994160075792081</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9987875377098668</v>
+        <v>0.9988008175769721</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9993628705314535</v>
+        <v>0.99936633736531</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6712356887424814</v>
+        <v>0.99936633736531</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.6685897361004693</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9988429929255541</v>
+        <v>0.9988591541715838</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9987875377098668</v>
+        <v>0.9988008175769721</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9992375606844266</v>
+        <v>0.999244360987668</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6574660622898086</v>
+        <v>0.999244360987668</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.6547527316865779</v>
       </c>
     </row>
     <row r="5">
@@ -533,40 +547,71 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9985279217658934</v>
+        <v>0.9985406712857549</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9993628705314535</v>
+        <v>0.99936633736531</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9992375606844266</v>
+        <v>0.999244360987668</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6654701192455768</v>
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.662866677809267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>Adj Close</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9985406712857549</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.99936633736531</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.999244360987668</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.662866677809267</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0.6669808006009431</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.6712356887424814</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.6574660622898086</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.6654701192455768</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="B7" t="n">
+        <v>0.6642954180740478</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6685897361004693</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.6547527316865779</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.662866677809267</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.662866677809267</v>
+      </c>
+      <c r="G7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>